<commit_message>
mere rapport Scrum kapitel + diverse
</commit_message>
<xml_diff>
--- a/Rapport/Excel ppt etc/Prisberegning.xlsx
+++ b/Rapport/Excel ppt etc/Prisberegning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\Dropbox\Datamekker\Hovedopgave\Excel ppt etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Documents\Afgangsprojekt-2014\Rapport\Excel ppt etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -95,10 +95,10 @@
     <t>Visning pr. download</t>
   </si>
   <si>
-    <t>CPM(DKK)</t>
-  </si>
-  <si>
     <t>CR(%)</t>
+  </si>
+  <si>
+    <t>eCPM(DKK)</t>
   </si>
 </sst>
 </file>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,37 +477,37 @@
         <v>21</v>
       </c>
       <c r="B4">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="C4">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="D4">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="E4">
-        <v>10000</v>
+        <v>1500</v>
       </c>
       <c r="F4">
-        <v>10000</v>
+        <v>1500</v>
       </c>
       <c r="G4">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="H4">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="I4">
-        <v>10000</v>
+        <v>250</v>
       </c>
       <c r="J4">
-        <v>10000</v>
+        <v>200</v>
       </c>
       <c r="K4">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="L4">
-        <v>10000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>SUM(B4:L4)</f>
-        <v>110000</v>
+        <v>16100</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -583,7 +583,7 @@
       </c>
       <c r="D11">
         <f>SUM(A11*B11*C11)</f>
-        <v>461999.99999999994</v>
+        <v>67620</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -611,7 +611,7 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15">
         <f>SUM(D11:D12)</f>
-        <v>554400</v>
+        <v>160020</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>22</v>
@@ -753,6 +753,16 @@
         <f>SUM(B19:L19)</f>
         <v>110000</v>
       </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <f>SUM((A23/1000)*B23*C23)</f>
+        <v>5280</v>
+      </c>
       <c r="E23" t="s">
         <v>3</v>
       </c>
@@ -890,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
nyt camera script, ny mojo, rettelser i rapport dokumenter
</commit_message>
<xml_diff>
--- a/Rapport/Excel ppt etc/Prisberegning.xlsx
+++ b/Rapport/Excel ppt etc/Prisberegning.xlsx
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,37 +660,37 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="C19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="D19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="E19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="F19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="G19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="H19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="I19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="J19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="K19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="L19">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -698,37 +698,37 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="C20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="D20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="G20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="H20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="I20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="J20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="K20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="L20">
-        <v>2000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -750,18 +750,17 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>SUM(B19:L19)</f>
-        <v>110000</v>
+        <v>6500000</v>
       </c>
       <c r="B23">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="D23">
         <f>SUM((A23/1000)*B23*C23)</f>
-        <v>5280</v>
+        <v>526500</v>
       </c>
       <c r="E23" t="s">
         <v>3</v>
@@ -769,14 +768,27 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>SUM(B20:L20)</f>
-        <v>22000</v>
+        <v>6500000</v>
+      </c>
+      <c r="B24">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <f>SUM((A24/1000)*B24*C24)</f>
+        <v>526500</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f>SUM(D23:D24)</f>
+        <v>1053000</v>
+      </c>
       <c r="E25" t="s">
         <v>8</v>
       </c>
@@ -914,8 +926,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>SUM(B29:L29)</f>
-        <v>1100000</v>
+        <v>2000000</v>
       </c>
       <c r="B33">
         <v>2.5000000000000001E-2</v>
@@ -925,7 +936,7 @@
       </c>
       <c r="D33">
         <f>SUM(A33*B33*C33)</f>
-        <v>275000</v>
+        <v>500000</v>
       </c>
       <c r="E33" t="s">
         <v>3</v>
@@ -933,8 +944,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>SUM(B30:L30)</f>
-        <v>1100000</v>
+        <v>2000000</v>
       </c>
       <c r="B34">
         <v>2.5000000000000001E-2</v>
@@ -944,7 +954,7 @@
       </c>
       <c r="D34">
         <f>SUM(A34*B34*C34)</f>
-        <v>275000</v>
+        <v>500000</v>
       </c>
       <c r="E34" t="s">
         <v>1</v>
@@ -953,7 +963,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D35">
         <f>SUM(D33:D34)</f>
-        <v>550000</v>
+        <v>1000000</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
i dont even know anymore... rettelser vel.
</commit_message>
<xml_diff>
--- a/Rapport/Excel ppt etc/Prisberegning.xlsx
+++ b/Rapport/Excel ppt etc/Prisberegning.xlsx
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,8 +572,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>SUM(B4:L4)</f>
-        <v>16100</v>
+        <v>120000</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -583,7 +582,7 @@
       </c>
       <c r="D11">
         <f>SUM(A11*B11*C11)</f>
-        <v>67620</v>
+        <v>503999.99999999994</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -591,8 +590,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>SUM(B5:L5)</f>
-        <v>22000</v>
+        <v>120000</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -602,18 +600,18 @@
       </c>
       <c r="D12">
         <f>SUM(A12*B12*C12)</f>
-        <v>92400</v>
+        <v>503999.99999999994</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13">
         <f>SUM(D11:D12)</f>
-        <v>160020</v>
-      </c>
-      <c r="E15" t="s">
+        <v>1007999.9999999999</v>
+      </c>
+      <c r="E13" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>